<commit_message>
minor updates to data dictionaries
</commit_message>
<xml_diff>
--- a/data_dictionary/data_description_units.xlsx
+++ b/data_dictionary/data_description_units.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aspeake\Documents\resstock\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EF4C4C3E-CF11-499B-AAE4-FD537F925187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D3B85D-C628-4E41-B841-A4A2C912C4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_description_units" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="480">
   <si>
     <t>field_name</t>
   </si>
@@ -1457,12 +1457,15 @@
   </si>
   <si>
     <t>in.puma</t>
+  </si>
+  <si>
+    <t>Not used</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1599,7 +1602,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1779,12 +1782,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1948,7 +1945,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2303,11 +2300,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3071,6 +3068,9 @@
       <c r="B69" t="s">
         <v>7</v>
       </c>
+      <c r="C69" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
@@ -3079,6 +3079,9 @@
       <c r="B70" t="s">
         <v>125</v>
       </c>
+      <c r="C70" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -3087,6 +3090,9 @@
       <c r="B71" t="s">
         <v>7</v>
       </c>
+      <c r="C71" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
@@ -3095,6 +3101,9 @@
       <c r="B72" t="s">
         <v>125</v>
       </c>
+      <c r="C72" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
@@ -3102,6 +3111,9 @@
       </c>
       <c r="B73" t="s">
         <v>7</v>
+      </c>
+      <c r="C73" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>